<commit_message>
Fix issues with INDs in ALP-leaning seats
</commit_message>
<xml_diff>
--- a/Ind-major preferencing.xlsx
+++ b/Ind-major preferencing.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{351A80D0-8BC0-47BA-8951-9335E177F441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAE8AD2-66AE-4039-A35F-ACA5DB3393C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="5310" windowWidth="24255" windowHeight="15300" activeTab="2" xr2:uid="{A68543AE-A11D-4AA7-B656-18DD4E512950}"/>
+    <workbookView xWindow="330" yWindow="4725" windowWidth="19800" windowHeight="14655" firstSheet="1" activeTab="3" xr2:uid="{A68543AE-A11D-4AA7-B656-18DD4E512950}"/>
   </bookViews>
   <sheets>
     <sheet name="LNP seat regression" sheetId="5" r:id="rId1"/>
-    <sheet name="ALP seat regression" sheetId="7" r:id="rId2"/>
+    <sheet name="ALP seat regression (fixed)" sheetId="11" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1305,7 +1304,7 @@
                   <c:v>38.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>27.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="75">
                   <c:v>49.8</c:v>
@@ -1440,7 +1439,7 @@
         <c:axId val="1201821168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="35"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4244,6 +4243,540 @@
           <c:orientation val="minMax"/>
           <c:max val="0.9"/>
           <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1201819920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Ind tcp vs Ind fp</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13731386701662293"/>
+                  <c:y val="-7.6523767862350543E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$AC$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>24.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>37.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>24.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$10:$AC$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>43.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.130000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>64.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>56.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>66.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>42.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>47.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-613D-4BFA-9789-91E7889548F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1201819920"/>
+        <c:axId val="1201821168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1201819920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1201821168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1201821168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4554,6 +5087,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6619,6 +7192,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7175,15 +8264,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>95251</xdr:colOff>
+      <xdr:colOff>219076</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>123825</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7319,6 +8408,49 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9EC8DE-8CF2-444D-9778-CEB9810B8063}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7627,7 +8759,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7878,17 +9010,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FAE203-CCF8-4F54-A5B6-DEF1D61C77A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EC6874-83EE-4929-8BE6-AD85DCC779A2}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7907,7 +9036,7 @@
         <v>155</v>
       </c>
       <c r="B4" s="2">
-        <v>0.39785415004805991</v>
+        <v>0.5756094786844822</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -7915,7 +9044,7 @@
         <v>156</v>
       </c>
       <c r="B5" s="2">
-        <v>0.15828792471046416</v>
+        <v>0.33132627195142134</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7923,7 +9052,7 @@
         <v>157</v>
       </c>
       <c r="B6" s="2">
-        <v>9.0950958687301298E-2</v>
+        <v>0.27783237370753505</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -7931,7 +9060,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="2">
-        <v>0.18587043066934741</v>
+        <v>0.10511474764894756</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7973,16 +9102,16 @@
         <v>2</v>
       </c>
       <c r="C12" s="2">
-        <v>0.16242199726919626</v>
+        <v>0.13687020771641156</v>
       </c>
       <c r="D12" s="2">
-        <v>8.1210998634598131E-2</v>
+        <v>6.8435103858205781E-2</v>
       </c>
       <c r="E12" s="2">
-        <v>2.3506839416556953</v>
+        <v>6.1937208322500217</v>
       </c>
       <c r="F12" s="2">
-        <v>0.11602310148593233</v>
+        <v>6.5339868071997986E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -7993,10 +9122,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="2">
-        <v>0.86369542493021689</v>
+        <v>0.27622775433254815</v>
       </c>
       <c r="D13" s="2">
-        <v>3.4547816997208679E-2</v>
+        <v>1.1049110173301926E-2</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -8009,7 +9138,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="3">
-        <v>1.0261174221994132</v>
+        <v>0.41309796204895971</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -8048,28 +9177,28 @@
         <v>163</v>
       </c>
       <c r="B17" s="2">
-        <v>-0.67420351633781839</v>
+        <v>0.24317948683282592</v>
       </c>
       <c r="C17" s="2">
-        <v>0.25347330944477814</v>
+        <v>0.14334600109378978</v>
       </c>
       <c r="D17" s="2">
-        <v>-2.6598599979407331</v>
+        <v>1.6964511390430497</v>
       </c>
       <c r="E17" s="2">
-        <v>1.3448234886622352E-2</v>
+        <v>0.10221927692165553</v>
       </c>
       <c r="F17" s="2">
-        <v>-1.1962415692333055</v>
+        <v>-5.2047128802850506E-2</v>
       </c>
       <c r="G17" s="2">
-        <v>-0.15216546344233128</v>
+        <v>0.53840610246850229</v>
       </c>
       <c r="H17" s="2">
-        <v>-1.1962415692333055</v>
+        <v>-5.2047128802850506E-2</v>
       </c>
       <c r="I17" s="2">
-        <v>-0.15216546344233128</v>
+        <v>0.53840610246850229</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -8077,28 +9206,28 @@
         <v>150</v>
       </c>
       <c r="B18" s="2">
-        <v>-4.7012398127806903E-3</v>
+        <v>-7.8756444780447091E-3</v>
       </c>
       <c r="C18" s="2">
-        <v>4.1409214796341116E-3</v>
+        <v>2.3418029150649002E-3</v>
       </c>
       <c r="D18" s="2">
-        <v>-1.1353124747480332</v>
+        <v>-3.3630688677430589</v>
       </c>
       <c r="E18" s="2">
-        <v>0.26701215779266668</v>
+        <v>2.4849084755171605E-3</v>
       </c>
       <c r="F18" s="2">
-        <v>-1.3229627244011371E-2</v>
+        <v>-1.2698677864570927E-2</v>
       </c>
       <c r="G18" s="2">
-        <v>3.8271476184499912E-3</v>
+        <v>-3.0526110915184909E-3</v>
       </c>
       <c r="H18" s="2">
-        <v>-1.3229627244011371E-2</v>
+        <v>-1.2698677864570927E-2</v>
       </c>
       <c r="I18" s="2">
-        <v>3.8271476184499912E-3</v>
+        <v>-3.0526110915184909E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8106,28 +9235,28 @@
         <v>176</v>
       </c>
       <c r="B19" s="3">
-        <v>1.6701354817676855E-2</v>
+        <v>1.0780678422470807E-2</v>
       </c>
       <c r="C19" s="3">
-        <v>7.7233284523503783E-3</v>
+        <v>4.3677507947617279E-3</v>
       </c>
       <c r="D19" s="3">
-        <v>2.1624555942061829</v>
+        <v>2.4682448539417918</v>
       </c>
       <c r="E19" s="3">
-        <v>4.0349838981965772E-2</v>
+        <v>2.0768625784034388E-2</v>
       </c>
       <c r="F19" s="3">
-        <v>7.9486211448479005E-4</v>
+        <v>1.7851272718401728E-3</v>
       </c>
       <c r="G19" s="3">
-        <v>3.260784752086892E-2</v>
+        <v>1.9776229573101441E-2</v>
       </c>
       <c r="H19" s="3">
-        <v>7.9486211448479005E-4</v>
+        <v>1.7851272718401728E-3</v>
       </c>
       <c r="I19" s="3">
-        <v>3.260784752086892E-2</v>
+        <v>1.9776229573101441E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8139,8 +9268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC942FC-F408-4DDC-937A-94949179FD9D}">
   <dimension ref="A1:DH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8149,6 +9278,8 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.7109375" customWidth="1"/>
     <col min="73" max="73" width="12.28515625" customWidth="1"/>
+    <col min="76" max="76" width="11.28515625" customWidth="1"/>
+    <col min="83" max="83" width="14.42578125" customWidth="1"/>
     <col min="90" max="90" width="12.28515625" customWidth="1"/>
     <col min="94" max="94" width="12.5703125" customWidth="1"/>
     <col min="95" max="95" width="11.85546875" customWidth="1"/>
@@ -9183,6 +10314,9 @@
       <c r="CZ5">
         <v>40.96</v>
       </c>
+      <c r="DA5">
+        <v>16.16</v>
+      </c>
       <c r="DB5">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -10528,7 +11662,7 @@
         <v>38.299999999999997</v>
       </c>
       <c r="BX10">
-        <v>27.5</v>
+        <v>38.5</v>
       </c>
       <c r="BY10">
         <v>49.8</v>
@@ -10855,7 +11989,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="BX11">
-        <v>38.5</v>
+        <v>27.5</v>
       </c>
       <c r="BY11">
         <v>42.6</v>
@@ -10937,6 +12071,9 @@
       </c>
       <c r="CZ11">
         <v>35.49</v>
+      </c>
+      <c r="DA11">
+        <v>34.700000000000003</v>
       </c>
       <c r="DB11">
         <f t="shared" si="3"/>
@@ -11275,7 +12412,7 @@
       </c>
       <c r="BX13">
         <f t="shared" si="10"/>
-        <v>0.14925373134328365</v>
+        <v>0.47761194029850768</v>
       </c>
       <c r="BY13">
         <f t="shared" si="10"/>
@@ -12133,7 +13270,7 @@
       </c>
       <c r="BX15">
         <f t="shared" si="18"/>
-        <v>0.65244444444444472</v>
+        <v>0.16355555555555579</v>
       </c>
       <c r="BY15">
         <f t="shared" si="18"/>
@@ -12562,7 +13699,7 @@
       </c>
       <c r="BX16">
         <f t="shared" si="22"/>
-        <v>0.10806944444444477</v>
+        <v>-0.38081944444444416</v>
       </c>
       <c r="BY16">
         <f t="shared" si="22"/>
@@ -12991,7 +14128,7 @@
       </c>
       <c r="BX17">
         <f t="shared" si="26"/>
-        <v>0.69635000000000014</v>
+        <v>0.48955000000000004</v>
       </c>
       <c r="BY17">
         <f t="shared" si="26"/>
@@ -13078,28 +14215,32 @@
         <v>0.43024000000000007</v>
       </c>
       <c r="CU17">
-        <f t="shared" si="27"/>
-        <v>0.55007000000000017</v>
+        <f t="shared" ref="CU17:CZ17" si="28">CU5*-0.00268+0.045033+CU11*0.01344</f>
+        <v>0.488429</v>
       </c>
       <c r="CV17">
-        <f t="shared" si="27"/>
-        <v>0.48699999999999999</v>
+        <f t="shared" si="28"/>
+        <v>0.42063299999999998</v>
       </c>
       <c r="CW17">
-        <f t="shared" si="27"/>
-        <v>0.6853100000000002</v>
+        <f t="shared" si="28"/>
+        <v>0.53534100000000007</v>
       </c>
       <c r="CX17">
-        <f t="shared" si="27"/>
-        <v>0.53456400000000015</v>
+        <f t="shared" si="28"/>
+        <v>0.40785220000000005</v>
       </c>
       <c r="CY17">
-        <f>CY5*-0.0081+0.8982+CY11*0.0188-0.7434</f>
-        <v>0.64304700000000004</v>
+        <f t="shared" si="28"/>
+        <v>0.51803660000000007</v>
       </c>
       <c r="CZ17">
-        <f>CZ5*-0.0081+0.8982+CZ11*0.0188-0.7434</f>
-        <v>0.49023600000000023</v>
+        <f t="shared" si="28"/>
+        <v>0.41224580000000005</v>
+      </c>
+      <c r="DA17">
+        <f>DA5*-0.00268+0.045033+DA11*0.01344</f>
+        <v>0.46809220000000007</v>
       </c>
       <c r="DB17">
         <f t="shared" si="3"/>
@@ -13127,347 +14268,347 @@
         <v>0.12966636321483771</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:BN18" si="28">C15-(0.0127*C11-0.034)</f>
+        <f t="shared" ref="C18:BN18" si="29">C15-(0.0127*C11-0.034)</f>
         <v>0.21947699166132162</v>
       </c>
       <c r="D18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.11196966340867442</v>
       </c>
       <c r="E18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.20758529774505297</v>
       </c>
       <c r="F18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.21330252389762583</v>
       </c>
       <c r="G18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.12654902076630603</v>
       </c>
       <c r="H18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>9.1873284566838631E-2</v>
       </c>
       <c r="I18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.28990908555783712</v>
       </c>
       <c r="J18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-3.8351053652230294E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-5.9633477558927839E-2</v>
       </c>
       <c r="L18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.259867974549328E-2</v>
       </c>
       <c r="M18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.10242639143730864</v>
       </c>
       <c r="N18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.3036214689265522E-2</v>
       </c>
       <c r="O18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.6278235294117795E-2</v>
       </c>
       <c r="P18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.16541851894669229</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>7.3233949432404688E-2</v>
       </c>
       <c r="R18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.1571439798125618E-2</v>
       </c>
       <c r="S18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-2.9432893203883759E-2</v>
       </c>
       <c r="T18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.14922092047853597</v>
       </c>
       <c r="U18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.10621719354838705</v>
       </c>
       <c r="V18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-8.8807014242115956E-2</v>
       </c>
       <c r="W18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.6363367913148408E-2</v>
       </c>
       <c r="X18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-6.5806732915079491E-2</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-3.0051414141413879E-2</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.12416953488372087</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.3633904041407963E-3</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>7.7927435897436059E-2</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.13539574370709373</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-4.4482649842259026E-4</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>8.4585890410959014E-2</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-9.3957162534435423E-2</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.12990723404255305</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.9380261437908469E-2</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.11439465753424649</v>
       </c>
       <c r="AJ18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-2.8100938967136058E-2</v>
       </c>
       <c r="AK18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-9.3897380073800607E-2</v>
       </c>
       <c r="AL18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-5.0422051282051406E-2</v>
       </c>
       <c r="AM18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-4.1882365887207673E-2</v>
       </c>
       <c r="AN18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.14224260223048346</v>
       </c>
       <c r="AO18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-6.5187883755588705E-2</v>
       </c>
       <c r="AP18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.155034632034635E-2</v>
       </c>
       <c r="AQ18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-5.6246077481840184E-2</v>
       </c>
       <c r="AR18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.0639520958082849E-3</v>
       </c>
       <c r="AS18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-5.7661164095371698E-2</v>
       </c>
       <c r="AT18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-8.0681404011461344E-2</v>
       </c>
       <c r="AU18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-2.0019999999999871E-2</v>
       </c>
       <c r="AV18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>2.6788080229226463E-2</v>
       </c>
       <c r="AW18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.8048874172185592E-2</v>
       </c>
       <c r="AX18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.205475113122084E-3</v>
       </c>
       <c r="AY18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.1149679538904898</v>
       </c>
       <c r="AZ18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-4.8179379844961456E-2</v>
       </c>
       <c r="BA18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.18594664082687337</v>
       </c>
       <c r="BB18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.2223376623375968E-3</v>
       </c>
       <c r="BC18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>5.2752920353982158E-2</v>
       </c>
       <c r="BD18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>8.3553722627737192E-2</v>
       </c>
       <c r="BE18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.10922294117647041</v>
       </c>
       <c r="BF18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6.4183333333333203E-2</v>
       </c>
       <c r="BG18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-3.8026067415730225E-2</v>
       </c>
       <c r="BH18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-6.1445820895522363E-2</v>
       </c>
       <c r="BI18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-2.7335471698113178E-2</v>
       </c>
       <c r="BJ18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-8.4603972602739663E-2</v>
       </c>
       <c r="BK18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.15198506849315074</v>
       </c>
       <c r="BL18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-0.21100252595155689</v>
       </c>
       <c r="BM18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.20735509433962274</v>
       </c>
       <c r="BN18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.11958760517306966</v>
       </c>
       <c r="BO18">
-        <f t="shared" ref="BO18:CJ18" si="29">BO15-(0.0127*BO11-0.034)</f>
+        <f t="shared" ref="BO18:CJ18" si="30">BO15-(0.0127*BO11-0.034)</f>
         <v>-0.12933514314115274</v>
       </c>
       <c r="BP18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-0.20592195121951204</v>
       </c>
       <c r="BQ18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.17147665332788864</v>
       </c>
       <c r="BR18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>9.4664955752212565E-2</v>
       </c>
       <c r="BS18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-4.9911132259638502E-3</v>
       </c>
       <c r="BT18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>5.6838709677420329E-4</v>
       </c>
       <c r="BU18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-8.3097652582160286E-3</v>
       </c>
       <c r="BV18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-6.9917651821862714E-2</v>
       </c>
       <c r="BW18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-4.1034576271186562E-2</v>
       </c>
       <c r="BX18">
-        <f t="shared" si="29"/>
-        <v>0.19749444444444475</v>
+        <f t="shared" si="30"/>
+        <v>-0.15169444444444424</v>
       </c>
       <c r="BY18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-0.12718129032258091</v>
       </c>
       <c r="BZ18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-0.19408171806167401</v>
       </c>
       <c r="CA18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-6.2012891566265105E-2</v>
       </c>
       <c r="CB18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1.4931938325991378E-2</v>
       </c>
       <c r="CC18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-1.9387448559670728E-2</v>
       </c>
       <c r="CD18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1.4000816326530774E-2</v>
       </c>
       <c r="CE18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>4.7453827160493733E-2</v>
       </c>
       <c r="CF18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.15412148936170211</v>
       </c>
       <c r="CG18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>-4.9234444444444525E-2</v>
       </c>
       <c r="CH18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.14122413793103472</v>
       </c>
       <c r="CI18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.17850777777777782</v>
       </c>
       <c r="CJ18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.15064781893004109</v>
       </c>
       <c r="DB18">
@@ -13763,7 +14904,7 @@
         <v>32</v>
       </c>
       <c r="DC34">
-        <f t="shared" ref="DC34:DC65" ca="1" si="30">OFFSET($B$5,0,DB34,1,1)</f>
+        <f t="shared" ref="DC34:DC65" ca="1" si="31">OFFSET($B$5,0,DB34,1,1)</f>
         <v>30.6</v>
       </c>
       <c r="DD34">
@@ -13781,7 +14922,7 @@
         <v>33</v>
       </c>
       <c r="DC35">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>29.2</v>
       </c>
       <c r="DD35">
@@ -13799,7 +14940,7 @@
         <v>34</v>
       </c>
       <c r="DC36">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>42.6</v>
       </c>
       <c r="DD36">
@@ -13817,7 +14958,7 @@
         <v>35</v>
       </c>
       <c r="DC37">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>27.1</v>
       </c>
       <c r="DD37">
@@ -13835,7 +14976,7 @@
         <v>36</v>
       </c>
       <c r="DC38">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>31.2</v>
       </c>
       <c r="DD38">
@@ -13853,7 +14994,7 @@
         <v>37</v>
       </c>
       <c r="DC39">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>72.7</v>
       </c>
       <c r="DD39">
@@ -13871,7 +15012,7 @@
         <v>38</v>
       </c>
       <c r="DC40">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>26.9</v>
       </c>
       <c r="DD40">
@@ -13889,7 +15030,7 @@
         <v>39</v>
       </c>
       <c r="DC41">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>67.099999999999994</v>
       </c>
       <c r="DD41">
@@ -13907,7 +15048,7 @@
         <v>40</v>
       </c>
       <c r="DC42">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>46.2</v>
       </c>
       <c r="DD42">
@@ -13925,7 +15066,7 @@
         <v>41</v>
       </c>
       <c r="DC43">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>41.3</v>
       </c>
       <c r="DD43">
@@ -13939,11 +15080,11 @@
     </row>
     <row r="44" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB44">
-        <f t="shared" ref="DB44:DB58" si="31">DB43+1</f>
+        <f t="shared" ref="DB44:DB58" si="32">DB43+1</f>
         <v>42</v>
       </c>
       <c r="DC44">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>33.4</v>
       </c>
       <c r="DD44">
@@ -13957,11 +15098,11 @@
     </row>
     <row r="45" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB45">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>43</v>
       </c>
       <c r="DC45">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>71.3</v>
       </c>
       <c r="DD45">
@@ -13975,11 +15116,11 @@
     </row>
     <row r="46" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB46">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>44</v>
       </c>
       <c r="DC46">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>69.8</v>
       </c>
       <c r="DD46">
@@ -13993,11 +15134,11 @@
     </row>
     <row r="47" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>45</v>
       </c>
       <c r="DC47">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>40</v>
       </c>
       <c r="DD47">
@@ -14011,11 +15152,11 @@
     </row>
     <row r="48" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>46</v>
       </c>
       <c r="DC48">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>34.9</v>
       </c>
       <c r="DD48">
@@ -14029,11 +15170,11 @@
     </row>
     <row r="49" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB49">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>47</v>
       </c>
       <c r="DC49">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>30.2</v>
       </c>
       <c r="DD49">
@@ -14047,11 +15188,11 @@
     </row>
     <row r="50" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB50">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>48</v>
       </c>
       <c r="DC50">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>44.2</v>
       </c>
       <c r="DD50">
@@ -14065,11 +15206,11 @@
     </row>
     <row r="51" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB51">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>49</v>
       </c>
       <c r="DC51">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>69.400000000000006</v>
       </c>
       <c r="DD51">
@@ -14083,11 +15224,11 @@
     </row>
     <row r="52" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB52">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>50</v>
       </c>
       <c r="DC52">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>25.8</v>
       </c>
       <c r="DD52">
@@ -14101,11 +15242,11 @@
     </row>
     <row r="53" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB53">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>51</v>
       </c>
       <c r="DC53">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>38.700000000000003</v>
       </c>
       <c r="DD53">
@@ -14119,11 +15260,11 @@
     </row>
     <row r="54" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB54">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>52</v>
       </c>
       <c r="DC54">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>38.5</v>
       </c>
       <c r="DD54">
@@ -14137,11 +15278,11 @@
     </row>
     <row r="55" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB55">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>53</v>
       </c>
       <c r="DC55">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>45.2</v>
       </c>
       <c r="DD55">
@@ -14155,11 +15296,11 @@
     </row>
     <row r="56" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB56">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>54</v>
       </c>
       <c r="DC56">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>27.4</v>
       </c>
       <c r="DD56">
@@ -14173,11 +15314,11 @@
     </row>
     <row r="57" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB57">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>55</v>
       </c>
       <c r="DC57">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>40.799999999999997</v>
       </c>
       <c r="DD57">
@@ -14191,11 +15332,11 @@
     </row>
     <row r="58" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB58">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>56</v>
       </c>
       <c r="DC58">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>36</v>
       </c>
       <c r="DD58">
@@ -14209,11 +15350,11 @@
     </row>
     <row r="59" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB59">
-        <f t="shared" ref="DB59:DB66" si="32">DB58+1</f>
+        <f t="shared" ref="DB59:DB66" si="33">DB58+1</f>
         <v>57</v>
       </c>
       <c r="DC59">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>35.6</v>
       </c>
       <c r="DD59">
@@ -14227,11 +15368,11 @@
     </row>
     <row r="60" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB60">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>58</v>
       </c>
       <c r="DC60">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>33.5</v>
       </c>
       <c r="DD60">
@@ -14245,11 +15386,11 @@
     </row>
     <row r="61" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB61">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>59</v>
       </c>
       <c r="DC61">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>31.8</v>
       </c>
       <c r="DD61">
@@ -14263,11 +15404,11 @@
     </row>
     <row r="62" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB62">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>60</v>
       </c>
       <c r="DC62">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>58.4</v>
       </c>
       <c r="DD62">
@@ -14281,11 +15422,11 @@
     </row>
     <row r="63" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB63">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>61</v>
       </c>
       <c r="DC63">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>29.2</v>
       </c>
       <c r="DD63">
@@ -14299,11 +15440,11 @@
     </row>
     <row r="64" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB64">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>62</v>
       </c>
       <c r="DC64">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>28.9</v>
       </c>
       <c r="DD64">
@@ -14317,11 +15458,11 @@
     </row>
     <row r="65" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB65">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>63</v>
       </c>
       <c r="DC65">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>26.5</v>
       </c>
       <c r="DD65">
@@ -14335,7 +15476,7 @@
     </row>
     <row r="66" spans="106:109" x14ac:dyDescent="0.25">
       <c r="DB66">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>64</v>
       </c>
       <c r="DC66">
@@ -14366,8 +15507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED575034-DF5C-4399-959D-FE713334FBF2}">
   <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14375,95 +15516,15 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" customWidth="1"/>
     <col min="31" max="31" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>101</v>
-      </c>
-      <c r="R1" t="s">
-        <v>109</v>
-      </c>
-      <c r="S1" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" t="s">
-        <v>117</v>
-      </c>
-      <c r="U1" t="s">
-        <v>118</v>
-      </c>
-      <c r="V1" t="s">
-        <v>119</v>
-      </c>
-      <c r="W1" t="s">
-        <v>125</v>
-      </c>
-      <c r="X1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>148</v>
-      </c>
       <c r="AF1" t="s">
         <v>150</v>
       </c>
@@ -14475,217 +15536,214 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S2" t="s">
+        <v>111</v>
+      </c>
+      <c r="T2" t="s">
+        <v>117</v>
+      </c>
+      <c r="U2" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" t="s">
+        <v>125</v>
+      </c>
+      <c r="X2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>148</v>
+      </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <f ca="1">OFFSET($B$4,0,AE2,1,1)</f>
+        <f ca="1">OFFSET($B$5,0,AE2,1,1)</f>
         <v>24.67</v>
       </c>
       <c r="AG2">
-        <f ca="1">OFFSET($B$10,0,AE2,1,1)</f>
+        <f ca="1">OFFSET($B$11,0,AE2,1,1)</f>
         <v>39.86</v>
       </c>
       <c r="AH2">
-        <f ca="1">OFFSET($B$14,0,AE2,1,1)</f>
+        <f ca="1">OFFSET($B$15,0,AE2,1,1)</f>
         <v>0.61418727199027134</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>20.149999999999999</v>
-      </c>
-      <c r="C3">
-        <v>11.42</v>
-      </c>
-      <c r="D3">
-        <v>22.65</v>
-      </c>
-      <c r="E3">
-        <v>23.23</v>
-      </c>
-      <c r="F3">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="G3">
-        <v>17.37</v>
-      </c>
-      <c r="H3">
-        <v>14.82</v>
-      </c>
-      <c r="I3">
-        <v>15.46</v>
-      </c>
-      <c r="J3">
-        <v>16.8</v>
-      </c>
-      <c r="K3">
-        <v>21</v>
-      </c>
-      <c r="L3">
-        <v>20.2</v>
-      </c>
-      <c r="M3">
-        <v>19.5</v>
-      </c>
-      <c r="N3">
-        <v>20.5</v>
-      </c>
-      <c r="O3">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="P3">
-        <v>21.6</v>
-      </c>
-      <c r="Q3">
-        <v>21.3</v>
-      </c>
-      <c r="R3">
-        <v>21.4</v>
-      </c>
-      <c r="S3">
-        <v>11.2</v>
-      </c>
-      <c r="T3">
-        <v>21</v>
-      </c>
-      <c r="U3">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="V3">
-        <v>18.5</v>
-      </c>
-      <c r="W3">
-        <v>19.2</v>
-      </c>
-      <c r="X3">
-        <v>36.5</v>
-      </c>
-      <c r="Y3">
-        <v>18.5</v>
-      </c>
-      <c r="Z3">
-        <v>20.7</v>
-      </c>
-      <c r="AA3">
-        <v>21.2</v>
-      </c>
-      <c r="AB3">
-        <v>14.3</v>
-      </c>
-      <c r="AC3">
-        <v>23.8</v>
-      </c>
       <c r="AE3">
         <f>AE2+1</f>
         <v>1</v>
       </c>
       <c r="AF3">
-        <f t="shared" ref="AF3:AF29" ca="1" si="0">OFFSET($B$4,0,AE3,1,1)</f>
+        <f t="shared" ref="AF3:AF29" ca="1" si="0">OFFSET($B$5,0,AE3,1,1)</f>
         <v>23.51</v>
       </c>
       <c r="AG3">
-        <f t="shared" ref="AG3:AG29" ca="1" si="1">OFFSET($B$10,0,AE3,1,1)</f>
+        <f t="shared" ref="AG3:AG29" ca="1" si="1">OFFSET($B$11,0,AE3,1,1)</f>
         <v>31.68</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH29" ca="1" si="2">OFFSET($B$15,0,AE3,1,1)</f>
-        <v>-0.23399384687367081</v>
+        <v>0.44564015312632915</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>24.67</v>
+        <v>20.149999999999999</v>
       </c>
       <c r="C4">
-        <v>23.51</v>
+        <v>11.42</v>
       </c>
       <c r="D4">
-        <v>21.26</v>
+        <v>22.65</v>
       </c>
       <c r="E4">
-        <v>38.08</v>
+        <v>23.23</v>
       </c>
       <c r="F4">
-        <v>44.07</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G4">
-        <v>50.05</v>
+        <v>17.37</v>
       </c>
       <c r="H4">
-        <v>25.88</v>
+        <v>14.82</v>
       </c>
       <c r="I4">
-        <v>53.53</v>
+        <v>15.46</v>
       </c>
       <c r="J4">
-        <v>42.5</v>
+        <v>16.8</v>
       </c>
       <c r="K4">
-        <v>20.399999999999999</v>
+        <v>21</v>
       </c>
       <c r="L4">
-        <v>29.5</v>
+        <v>20.2</v>
       </c>
       <c r="M4">
-        <v>30.3</v>
+        <v>19.5</v>
       </c>
       <c r="N4">
-        <v>26.6</v>
+        <v>20.5</v>
       </c>
       <c r="O4">
-        <v>24.1</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="P4">
-        <v>39.6</v>
+        <v>21.6</v>
       </c>
       <c r="Q4">
-        <v>38.5</v>
+        <v>21.3</v>
       </c>
       <c r="R4">
-        <v>37.299999999999997</v>
+        <v>21.4</v>
       </c>
       <c r="S4">
-        <v>26.9</v>
+        <v>11.2</v>
       </c>
       <c r="T4">
-        <v>30.6</v>
+        <v>21</v>
       </c>
       <c r="U4">
-        <v>46</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="V4">
-        <v>25.9</v>
+        <v>18.5</v>
       </c>
       <c r="W4">
-        <v>25.1</v>
+        <v>19.2</v>
       </c>
       <c r="X4">
-        <v>37.700000000000003</v>
+        <v>36.5</v>
       </c>
       <c r="Y4">
-        <v>45.2</v>
+        <v>18.5</v>
       </c>
       <c r="Z4">
-        <v>24.6</v>
+        <v>20.7</v>
       </c>
       <c r="AA4">
-        <v>22.7</v>
+        <v>21.2</v>
       </c>
       <c r="AB4">
-        <v>21.4</v>
+        <v>14.3</v>
       </c>
       <c r="AC4">
-        <v>24.1</v>
+        <v>23.8</v>
       </c>
       <c r="AE4">
-        <f t="shared" ref="AE4:AE29" si="3">AE3+1</f>
+        <f t="shared" ref="AE4:AE30" si="3">AE3+1</f>
         <v>2</v>
       </c>
       <c r="AF4">
@@ -14698,96 +15756,99 @@
       </c>
       <c r="AH4">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.36174646472248362</v>
+        <v>0.33273753527751637</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>40.369999999999997</v>
+        <v>24.67</v>
       </c>
       <c r="C5">
-        <v>37.74</v>
+        <v>23.51</v>
       </c>
       <c r="D5">
-        <v>35.79</v>
+        <v>21.26</v>
       </c>
       <c r="E5">
-        <v>24.75</v>
+        <v>38.08</v>
       </c>
       <c r="F5">
-        <v>23.01</v>
+        <v>44.07</v>
       </c>
       <c r="G5">
-        <v>20.22</v>
+        <v>50.05</v>
       </c>
       <c r="H5">
-        <v>49.88</v>
+        <v>25.88</v>
       </c>
       <c r="I5">
-        <v>21.43</v>
+        <v>53.53</v>
       </c>
       <c r="J5">
-        <v>30.7</v>
+        <v>42.5</v>
       </c>
       <c r="K5">
-        <v>40.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="L5">
-        <v>35.6</v>
+        <v>29.5</v>
       </c>
       <c r="M5">
-        <v>40.5</v>
+        <v>30.3</v>
       </c>
       <c r="N5">
-        <v>39.700000000000003</v>
+        <v>26.6</v>
       </c>
       <c r="O5">
-        <v>31.2</v>
+        <v>24.1</v>
       </c>
       <c r="P5">
-        <v>20</v>
+        <v>39.6</v>
       </c>
       <c r="Q5">
-        <v>22.8</v>
+        <v>38.5</v>
       </c>
       <c r="R5">
-        <v>31.9</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="S5">
-        <v>45.4</v>
+        <v>26.9</v>
       </c>
       <c r="T5">
-        <v>32.799999999999997</v>
+        <v>30.6</v>
       </c>
       <c r="U5">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="V5">
-        <v>47</v>
+        <v>25.9</v>
       </c>
       <c r="W5">
-        <v>43.6</v>
+        <v>25.1</v>
       </c>
       <c r="X5">
-        <v>18.5</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="Y5">
-        <v>26.4</v>
+        <v>45.2</v>
       </c>
       <c r="Z5">
-        <v>41</v>
+        <v>24.6</v>
       </c>
       <c r="AA5">
-        <v>56.1</v>
+        <v>22.7</v>
       </c>
       <c r="AB5">
-        <v>45.3</v>
+        <v>21.4</v>
       </c>
       <c r="AC5">
-        <v>43.8</v>
+        <v>24.1</v>
+      </c>
+      <c r="AD5">
+        <v>16.16</v>
       </c>
       <c r="AE5">
         <f t="shared" si="3"/>
@@ -14803,96 +15864,96 @@
       </c>
       <c r="AH5">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.23510015126050393</v>
+        <v>0.34837184873949606</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>9.49</v>
+        <v>40.369999999999997</v>
       </c>
       <c r="C6">
-        <v>12.94</v>
+        <v>37.74</v>
       </c>
       <c r="D6">
-        <v>18.98</v>
+        <v>35.79</v>
       </c>
       <c r="E6">
-        <v>7.92</v>
+        <v>24.75</v>
       </c>
       <c r="F6">
-        <v>10.6</v>
+        <v>23.01</v>
       </c>
       <c r="G6">
-        <v>9.57</v>
+        <v>20.22</v>
       </c>
       <c r="H6">
-        <v>5.04</v>
+        <v>49.88</v>
       </c>
       <c r="I6">
-        <v>5.03</v>
+        <v>21.43</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>30.7</v>
       </c>
       <c r="K6">
-        <v>9.5</v>
+        <v>40.4</v>
       </c>
       <c r="L6">
-        <v>9.6</v>
+        <v>35.6</v>
       </c>
       <c r="M6">
-        <v>5.7</v>
+        <v>40.5</v>
       </c>
       <c r="N6">
-        <v>5</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="O6">
-        <v>11.2</v>
+        <v>31.2</v>
       </c>
       <c r="P6">
-        <v>15.6</v>
+        <v>20</v>
       </c>
       <c r="Q6">
-        <v>14.1</v>
+        <v>22.8</v>
       </c>
       <c r="R6">
-        <v>5.9</v>
+        <v>31.9</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>45.4</v>
       </c>
       <c r="T6">
-        <v>4.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="U6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="V6">
-        <v>3.6</v>
+        <v>47</v>
       </c>
       <c r="W6">
-        <v>6.6</v>
+        <v>43.6</v>
       </c>
       <c r="X6">
-        <v>3.1</v>
+        <v>18.5</v>
       </c>
       <c r="Y6">
-        <v>3.4</v>
+        <v>26.4</v>
       </c>
       <c r="Z6">
-        <v>3.4</v>
+        <v>41</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <v>56.1</v>
       </c>
       <c r="AB6">
-        <v>5.6</v>
+        <v>45.3</v>
       </c>
       <c r="AC6">
-        <v>6</v>
+        <v>43.8</v>
       </c>
       <c r="AE6">
         <f t="shared" si="3"/>
@@ -14908,124 +15969,96 @@
       </c>
       <c r="AH6">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.28457789108236908</v>
+        <v>0.25936010891763095</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:N7" si="4">100-SUM(B3:B6)</f>
-        <v>5.3200000000000074</v>
+        <v>9.49</v>
       </c>
       <c r="C7">
-        <f t="shared" si="4"/>
-        <v>14.39</v>
+        <v>12.94</v>
       </c>
       <c r="D7">
-        <f t="shared" si="4"/>
-        <v>1.3200000000000074</v>
+        <v>18.98</v>
       </c>
       <c r="E7">
-        <f t="shared" si="4"/>
-        <v>6.019999999999996</v>
+        <v>7.92</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
-        <v>2.4200000000000017</v>
+        <v>10.6</v>
       </c>
       <c r="G7">
-        <f t="shared" si="4"/>
-        <v>2.789999999999992</v>
+        <v>9.57</v>
       </c>
       <c r="H7">
-        <f t="shared" si="4"/>
-        <v>4.3799999999999812</v>
+        <v>5.04</v>
       </c>
       <c r="I7">
-        <f t="shared" si="4"/>
-        <v>4.5499999999999829</v>
+        <v>5.03</v>
       </c>
       <c r="J7">
-        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K7">
-        <f t="shared" si="4"/>
-        <v>8.7000000000000028</v>
+        <v>9.5</v>
       </c>
       <c r="L7">
-        <f t="shared" si="4"/>
-        <v>5.0999999999999943</v>
+        <v>9.6</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5.7</v>
       </c>
       <c r="N7">
-        <f t="shared" si="4"/>
-        <v>8.1999999999999886</v>
+        <v>5</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:W7" si="5">100-SUM(O3:O6)</f>
-        <v>23.699999999999989</v>
+        <v>11.2</v>
       </c>
       <c r="P7">
-        <f t="shared" si="5"/>
-        <v>3.2000000000000028</v>
+        <v>15.6</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="5"/>
-        <v>3.3000000000000114</v>
+        <v>14.1</v>
       </c>
       <c r="R7">
-        <f t="shared" si="5"/>
-        <v>3.5</v>
+        <v>5.9</v>
       </c>
       <c r="S7">
-        <f t="shared" si="5"/>
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="5"/>
-        <v>10.799999999999997</v>
+        <v>4.8</v>
       </c>
       <c r="U7">
-        <f t="shared" si="5"/>
-        <v>2.7000000000000028</v>
+        <v>3</v>
       </c>
       <c r="V7">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="W7">
-        <f t="shared" si="5"/>
-        <v>5.5</v>
+        <v>6.6</v>
       </c>
       <c r="X7">
-        <f t="shared" ref="X7:AC7" si="6">100-SUM(X3:X6)</f>
-        <v>4.2000000000000028</v>
+        <v>3.1</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="6"/>
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="6"/>
-        <v>10.299999999999997</v>
+        <v>3.4</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="6"/>
-        <v>13.400000000000006</v>
+        <v>5.6</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="6"/>
-        <v>2.2999999999999972</v>
+        <v>6</v>
       </c>
       <c r="AE7">
         <f t="shared" si="3"/>
@@ -15041,10 +16074,125 @@
       </c>
       <c r="AH7">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.2417127572427572</v>
+        <v>0.26275724275724277</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:N8" si="4">100-SUM(B4:B7)</f>
+        <v>5.3200000000000074</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="4"/>
+        <v>14.39</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="4"/>
+        <v>1.3200000000000074</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>6.019999999999996</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>2.4200000000000017</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>2.789999999999992</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>4.3799999999999812</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>4.5499999999999829</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="4"/>
+        <v>8.7000000000000028</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>5.0999999999999943</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>8.1999999999999886</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:W8" si="5">100-SUM(O4:O7)</f>
+        <v>23.699999999999989</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>3.2000000000000028</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>3.3000000000000114</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="5"/>
+        <v>16.5</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="5"/>
+        <v>10.799999999999997</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="5"/>
+        <v>2.7000000000000028</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="5"/>
+        <v>5.5</v>
+      </c>
+      <c r="X8">
+        <f t="shared" ref="X8:AC8" si="6">100-SUM(X4:X7)</f>
+        <v>4.2000000000000028</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="6"/>
+        <v>6.5</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="6"/>
+        <v>10.299999999999997</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="6"/>
+        <v>13.400000000000006</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="6"/>
+        <v>2.2999999999999972</v>
+      </c>
       <c r="AE8">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -15059,97 +16207,10 @@
       </c>
       <c r="AH8">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.41468751777434276</v>
+        <v>0.24930448222565724</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>43.77</v>
-      </c>
-      <c r="C9">
-        <v>41.42</v>
-      </c>
-      <c r="D9">
-        <v>51.21</v>
-      </c>
-      <c r="E9">
-        <v>65.510000000000005</v>
-      </c>
-      <c r="F9">
-        <v>67.78</v>
-      </c>
-      <c r="G9">
-        <v>72.12</v>
-      </c>
-      <c r="H9">
-        <v>37.130000000000003</v>
-      </c>
-      <c r="I9">
-        <v>72.11</v>
-      </c>
-      <c r="J9">
-        <v>60.7</v>
-      </c>
-      <c r="K9">
-        <v>41.1</v>
-      </c>
-      <c r="L9">
-        <v>49.1</v>
-      </c>
-      <c r="M9">
-        <v>50.1</v>
-      </c>
-      <c r="N9">
-        <v>48</v>
-      </c>
-      <c r="O9">
-        <v>48.8</v>
-      </c>
-      <c r="P9">
-        <v>66.599999999999994</v>
-      </c>
-      <c r="Q9">
-        <v>64.7</v>
-      </c>
-      <c r="R9">
-        <v>59.8</v>
-      </c>
-      <c r="S9">
-        <v>42.1</v>
-      </c>
-      <c r="T9">
-        <v>56.1</v>
-      </c>
-      <c r="U9">
-        <v>58.2</v>
-      </c>
-      <c r="V9">
-        <v>42.6</v>
-      </c>
-      <c r="W9">
-        <v>42.6</v>
-      </c>
-      <c r="X9">
-        <v>58.2</v>
-      </c>
-      <c r="Y9">
-        <v>66.7</v>
-      </c>
-      <c r="Z9">
-        <v>50.6</v>
-      </c>
-      <c r="AA9">
-        <v>40.5</v>
-      </c>
-      <c r="AB9">
-        <v>42.8</v>
-      </c>
-      <c r="AC9">
-        <v>47.4</v>
-      </c>
       <c r="AE9">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -15164,96 +16225,96 @@
       </c>
       <c r="AH9">
         <f t="shared" ca="1" si="2"/>
-        <v>-3.5228882122174288E-2</v>
+        <v>0.4462731178778257</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>39.86</v>
+        <v>43.77</v>
       </c>
       <c r="C10">
-        <v>31.68</v>
+        <v>41.42</v>
       </c>
       <c r="D10">
-        <v>34.18</v>
+        <v>51.21</v>
       </c>
       <c r="E10">
-        <v>41.09</v>
+        <v>65.510000000000005</v>
       </c>
       <c r="F10">
-        <v>34.659999999999997</v>
+        <v>67.78</v>
       </c>
       <c r="G10">
-        <v>33.83</v>
+        <v>72.12</v>
       </c>
       <c r="H10">
-        <v>24.47</v>
+        <v>37.130000000000003</v>
       </c>
       <c r="I10">
-        <v>42.63</v>
+        <v>72.11</v>
       </c>
       <c r="J10">
-        <v>36.799999999999997</v>
+        <v>60.7</v>
       </c>
       <c r="K10">
-        <v>36.6</v>
+        <v>41.1</v>
       </c>
       <c r="L10">
-        <v>41.1</v>
+        <v>49.1</v>
       </c>
       <c r="M10">
-        <v>35</v>
+        <v>50.1</v>
       </c>
       <c r="N10">
-        <v>40.299999999999997</v>
+        <v>48</v>
       </c>
       <c r="O10">
-        <v>32.200000000000003</v>
+        <v>48.8</v>
       </c>
       <c r="P10">
-        <v>43.1</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="Q10">
-        <v>39.1</v>
+        <v>64.7</v>
       </c>
       <c r="R10">
-        <v>38.299999999999997</v>
+        <v>59.8</v>
       </c>
       <c r="S10">
-        <v>27.9</v>
+        <v>42.1</v>
       </c>
       <c r="T10">
-        <v>39</v>
+        <v>56.1</v>
       </c>
       <c r="U10">
-        <v>38.9</v>
+        <v>58.2</v>
       </c>
       <c r="V10">
-        <v>34.799999999999997</v>
+        <v>42.6</v>
       </c>
       <c r="W10">
-        <v>34.799999999999997</v>
+        <v>42.6</v>
       </c>
       <c r="X10">
-        <v>49.9</v>
+        <v>58.2</v>
       </c>
       <c r="Y10">
-        <v>40.6</v>
+        <v>66.7</v>
       </c>
       <c r="Z10">
-        <v>34.799999999999997</v>
+        <v>50.6</v>
       </c>
       <c r="AA10">
-        <v>28.9</v>
+        <v>40.5</v>
       </c>
       <c r="AB10">
-        <v>32.1</v>
+        <v>42.8</v>
       </c>
       <c r="AC10">
-        <v>38.200000000000003</v>
+        <v>47.4</v>
       </c>
       <c r="AE10">
         <f t="shared" si="3"/>
@@ -15269,10 +16330,100 @@
       </c>
       <c r="AH10">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.16606470588235306</v>
+        <v>0.38823529411764696</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>39.86</v>
+      </c>
+      <c r="C11">
+        <v>31.68</v>
+      </c>
+      <c r="D11">
+        <v>34.18</v>
+      </c>
+      <c r="E11">
+        <v>41.09</v>
+      </c>
+      <c r="F11">
+        <v>34.659999999999997</v>
+      </c>
+      <c r="G11">
+        <v>33.83</v>
+      </c>
+      <c r="H11">
+        <v>24.47</v>
+      </c>
+      <c r="I11">
+        <v>42.63</v>
+      </c>
+      <c r="J11">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="K11">
+        <v>36.6</v>
+      </c>
+      <c r="L11">
+        <v>41.1</v>
+      </c>
+      <c r="M11">
+        <v>35</v>
+      </c>
+      <c r="N11">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="O11">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="P11">
+        <v>43.1</v>
+      </c>
+      <c r="Q11">
+        <v>39.1</v>
+      </c>
+      <c r="R11">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="S11">
+        <v>27.9</v>
+      </c>
+      <c r="T11">
+        <v>39</v>
+      </c>
+      <c r="U11">
+        <v>38.9</v>
+      </c>
+      <c r="V11">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="W11">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="X11">
+        <v>49.9</v>
+      </c>
+      <c r="Y11">
+        <v>40.6</v>
+      </c>
+      <c r="Z11">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="AA11">
+        <v>28.9</v>
+      </c>
+      <c r="AB11">
+        <v>32.1</v>
+      </c>
+      <c r="AC11">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="AD11">
+        <v>34.700000000000003</v>
+      </c>
       <c r="AE11">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -15287,125 +16438,10 @@
       </c>
       <c r="AH11">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.24182666666666658</v>
+        <v>0.45833333333333343</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <f t="shared" ref="B12:I12" si="7">(B9-B4)/SUM(B5:B7)</f>
-        <v>0.34613990576295756</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="7"/>
-        <v>0.27524204702627941</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="7"/>
-        <v>0.53396327331075055</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="7"/>
-        <v>0.70896872576893277</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="7"/>
-        <v>0.65806272550652234</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="7"/>
-        <v>0.67740945365254801</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="7"/>
-        <v>0.18971332209106251</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="7"/>
-        <v>0.59916156078684324</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ref="J12:AC12" si="8">(J9-J4)/SUM(J5:J7)</f>
-        <v>0.44717444717444721</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="8"/>
-        <v>0.35324232081911267</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="8"/>
-        <v>0.38966202783300202</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="8"/>
-        <v>0.39442231075697209</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="8"/>
-        <v>0.40453686200378075</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="8"/>
-        <v>0.37367624810892586</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
-        <v>0.69587628865979356</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="8"/>
-        <v>0.65174129353233823</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="8"/>
-        <v>0.5447941888619855</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="8"/>
-        <v>0.24555735056542816</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="8"/>
-        <v>0.52685950413223148</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="8"/>
-        <v>0.77707006369426757</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="8"/>
-        <v>0.30035971223021585</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="8"/>
-        <v>0.31418312387791741</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="8"/>
-        <v>0.79457364341085257</v>
-      </c>
-      <c r="Y12">
-        <f t="shared" si="8"/>
-        <v>0.59228650137741057</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="8"/>
-        <v>0.47531992687385743</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="8"/>
-        <v>0.31729055258467026</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="8"/>
-        <v>0.33281493001555201</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="8"/>
-        <v>0.44721689059500958</v>
-      </c>
       <c r="AE12">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -15420,124 +16456,124 @@
       </c>
       <c r="AH12">
         <f t="shared" ca="1" si="2"/>
-        <v>-8.315084745762702E-2</v>
+        <v>0.55694915254237298</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:I13" si="9">B6*0.2+B7*0.5</f>
-        <v>4.5580000000000034</v>
+        <f t="shared" ref="B13:I13" si="7">(B10-B5)/SUM(B6:B8)</f>
+        <v>0.34613990576295756</v>
       </c>
       <c r="C13">
-        <f t="shared" si="9"/>
-        <v>9.7830000000000013</v>
+        <f t="shared" si="7"/>
+        <v>0.27524204702627941</v>
       </c>
       <c r="D13">
-        <f t="shared" si="9"/>
-        <v>4.456000000000004</v>
+        <f t="shared" si="7"/>
+        <v>0.53396327331075055</v>
       </c>
       <c r="E13">
-        <f t="shared" si="9"/>
-        <v>4.5939999999999976</v>
+        <f t="shared" si="7"/>
+        <v>0.70896872576893277</v>
       </c>
       <c r="F13">
-        <f t="shared" si="9"/>
-        <v>3.330000000000001</v>
+        <f t="shared" si="7"/>
+        <v>0.65806272550652234</v>
       </c>
       <c r="G13">
-        <f t="shared" si="9"/>
-        <v>3.3089999999999962</v>
+        <f t="shared" si="7"/>
+        <v>0.67740945365254801</v>
       </c>
       <c r="H13">
-        <f t="shared" si="9"/>
-        <v>3.1979999999999906</v>
+        <f t="shared" si="7"/>
+        <v>0.18971332209106251</v>
       </c>
       <c r="I13">
-        <f t="shared" si="9"/>
-        <v>3.2809999999999917</v>
+        <f t="shared" si="7"/>
+        <v>0.59916156078684324</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:AC13" si="10">J6*0.2+J7*0.5</f>
-        <v>3.5</v>
+        <f t="shared" ref="J13:AC13" si="8">(J10-J5)/SUM(J6:J8)</f>
+        <v>0.44717444717444721</v>
       </c>
       <c r="K13">
-        <f t="shared" si="10"/>
-        <v>6.2500000000000018</v>
+        <f t="shared" si="8"/>
+        <v>0.35324232081911267</v>
       </c>
       <c r="L13">
-        <f t="shared" si="10"/>
-        <v>4.4699999999999971</v>
+        <f t="shared" si="8"/>
+        <v>0.38966202783300202</v>
       </c>
       <c r="M13">
-        <f t="shared" si="10"/>
-        <v>3.14</v>
+        <f t="shared" si="8"/>
+        <v>0.39442231075697209</v>
       </c>
       <c r="N13">
-        <f t="shared" si="10"/>
-        <v>5.0999999999999943</v>
+        <f t="shared" si="8"/>
+        <v>0.40453686200378075</v>
       </c>
       <c r="O13">
-        <f t="shared" si="10"/>
-        <v>14.089999999999995</v>
+        <f t="shared" si="8"/>
+        <v>0.37367624810892586</v>
       </c>
       <c r="P13">
-        <f t="shared" si="10"/>
-        <v>4.7200000000000015</v>
+        <f t="shared" si="8"/>
+        <v>0.69587628865979356</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="10"/>
-        <v>4.470000000000006</v>
+        <f t="shared" si="8"/>
+        <v>0.65174129353233823</v>
       </c>
       <c r="R13">
-        <f t="shared" si="10"/>
-        <v>2.93</v>
+        <f t="shared" si="8"/>
+        <v>0.5447941888619855</v>
       </c>
       <c r="S13">
-        <f t="shared" si="10"/>
-        <v>8.25</v>
+        <f t="shared" si="8"/>
+        <v>0.24555735056542816</v>
       </c>
       <c r="T13">
-        <f t="shared" si="10"/>
-        <v>6.3599999999999985</v>
+        <f t="shared" si="8"/>
+        <v>0.52685950413223148</v>
       </c>
       <c r="U13">
-        <f t="shared" si="10"/>
-        <v>1.9500000000000015</v>
+        <f t="shared" si="8"/>
+        <v>0.77707006369426757</v>
       </c>
       <c r="V13">
-        <f t="shared" si="10"/>
-        <v>3.22</v>
+        <f t="shared" si="8"/>
+        <v>0.30035971223021585</v>
       </c>
       <c r="W13">
-        <f t="shared" si="10"/>
-        <v>4.07</v>
+        <f t="shared" si="8"/>
+        <v>0.31418312387791741</v>
       </c>
       <c r="X13">
-        <f t="shared" si="10"/>
-        <v>2.7200000000000015</v>
+        <f t="shared" si="8"/>
+        <v>0.79457364341085257</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="10"/>
-        <v>3.93</v>
+        <f t="shared" si="8"/>
+        <v>0.59228650137741057</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="10"/>
-        <v>5.8299999999999983</v>
+        <f t="shared" si="8"/>
+        <v>0.47531992687385743</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>0.31729055258467026</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="10"/>
-        <v>7.8200000000000029</v>
+        <f t="shared" si="8"/>
+        <v>0.33281493001555201</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="10"/>
-        <v>2.3499999999999988</v>
+        <f t="shared" si="8"/>
+        <v>0.44721689059500958</v>
       </c>
       <c r="AE13">
         <f t="shared" si="3"/>
@@ -15553,124 +16589,124 @@
       </c>
       <c r="AH13">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.22689920792079205</v>
+        <v>0.40792079207920789</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:AC14" si="11">(B10-B13-B3)/B4</f>
-        <v>0.61418727199027134</v>
+        <f t="shared" ref="B14:I14" si="9">B7*0.2+B8*0.5</f>
+        <v>4.5580000000000034</v>
       </c>
       <c r="C14">
-        <f t="shared" si="11"/>
-        <v>0.44564015312632915</v>
+        <f t="shared" si="9"/>
+        <v>9.7830000000000013</v>
       </c>
       <c r="D14">
-        <f t="shared" si="11"/>
-        <v>0.33273753527751637</v>
+        <f t="shared" si="9"/>
+        <v>4.456000000000004</v>
       </c>
       <c r="E14">
-        <f t="shared" si="11"/>
-        <v>0.34837184873949606</v>
+        <f t="shared" si="9"/>
+        <v>4.5939999999999976</v>
       </c>
       <c r="F14">
-        <f t="shared" si="11"/>
-        <v>0.25936010891763095</v>
+        <f t="shared" si="9"/>
+        <v>3.330000000000001</v>
       </c>
       <c r="G14">
-        <f t="shared" si="11"/>
-        <v>0.26275724275724277</v>
+        <f t="shared" si="9"/>
+        <v>3.3089999999999962</v>
       </c>
       <c r="H14">
-        <f t="shared" si="11"/>
-        <v>0.24930448222565724</v>
+        <f t="shared" si="9"/>
+        <v>3.1979999999999906</v>
       </c>
       <c r="I14">
-        <f t="shared" si="11"/>
-        <v>0.4462731178778257</v>
+        <f t="shared" si="9"/>
+        <v>3.2809999999999917</v>
       </c>
       <c r="J14">
-        <f t="shared" si="11"/>
-        <v>0.38823529411764696</v>
+        <f t="shared" ref="J14:AC14" si="10">J7*0.2+J8*0.5</f>
+        <v>3.5</v>
       </c>
       <c r="K14">
-        <f t="shared" si="11"/>
-        <v>0.45833333333333343</v>
+        <f t="shared" si="10"/>
+        <v>6.2500000000000018</v>
       </c>
       <c r="L14">
-        <f t="shared" si="11"/>
-        <v>0.55694915254237298</v>
+        <f t="shared" si="10"/>
+        <v>4.4699999999999971</v>
       </c>
       <c r="M14">
-        <f t="shared" si="11"/>
-        <v>0.40792079207920789</v>
+        <f t="shared" si="10"/>
+        <v>3.14</v>
       </c>
       <c r="N14">
-        <f t="shared" si="11"/>
-        <v>0.55263157894736847</v>
+        <f t="shared" si="10"/>
+        <v>5.0999999999999943</v>
       </c>
       <c r="O14">
-        <f t="shared" si="11"/>
-        <v>0.34481327800829897</v>
+        <f t="shared" si="10"/>
+        <v>14.089999999999995</v>
       </c>
       <c r="P14">
-        <f t="shared" si="11"/>
-        <v>0.42373737373737375</v>
+        <f t="shared" si="10"/>
+        <v>4.7200000000000015</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="11"/>
-        <v>0.34623376623376612</v>
+        <f t="shared" si="10"/>
+        <v>4.470000000000006</v>
       </c>
       <c r="R14">
-        <f t="shared" si="11"/>
-        <v>0.37453083109919572</v>
+        <f t="shared" si="10"/>
+        <v>2.93</v>
       </c>
       <c r="S14">
-        <f t="shared" si="11"/>
-        <v>0.31412639405204462</v>
+        <f t="shared" si="10"/>
+        <v>8.25</v>
       </c>
       <c r="T14">
-        <f t="shared" si="11"/>
-        <v>0.38039215686274508</v>
+        <f t="shared" si="10"/>
+        <v>6.3599999999999985</v>
       </c>
       <c r="U14">
-        <f t="shared" si="11"/>
-        <v>-2.9347826086956554E-2</v>
+        <f t="shared" si="10"/>
+        <v>1.9500000000000015</v>
       </c>
       <c r="V14">
-        <f t="shared" si="11"/>
-        <v>0.50501930501930503</v>
+        <f t="shared" si="10"/>
+        <v>3.22</v>
       </c>
       <c r="W14">
-        <f t="shared" si="11"/>
-        <v>0.45936254980079672</v>
+        <f t="shared" si="10"/>
+        <v>4.07</v>
       </c>
       <c r="X14">
-        <f t="shared" si="11"/>
-        <v>0.28328912466843498</v>
+        <f t="shared" si="10"/>
+        <v>2.7200000000000015</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="11"/>
-        <v>0.40199115044247791</v>
+        <f t="shared" si="10"/>
+        <v>3.93</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="11"/>
-        <v>0.33617886178861783</v>
+        <f t="shared" si="10"/>
+        <v>5.8299999999999983</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="11"/>
-        <v>0.33920704845814975</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="11"/>
-        <v>0.46635514018691576</v>
+        <f t="shared" si="10"/>
+        <v>7.8200000000000029</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
+        <f t="shared" si="10"/>
+        <v>2.3499999999999988</v>
       </c>
       <c r="AE14">
         <f t="shared" si="3"/>
@@ -15686,124 +16722,124 @@
       </c>
       <c r="AH14">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.10660842105263146</v>
+        <v>0.55263157894736847</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:AC15" si="12">B14-((-0.0066*B4)+0.8348)</f>
-        <v>-5.779072800972862E-2</v>
+        <f t="shared" ref="B15:AC15" si="11">(B11-B14-B4)/B5</f>
+        <v>0.61418727199027134</v>
       </c>
       <c r="C15">
-        <f t="shared" si="12"/>
-        <v>-0.23399384687367081</v>
+        <f t="shared" si="11"/>
+        <v>0.44564015312632915</v>
       </c>
       <c r="D15">
-        <f t="shared" si="12"/>
-        <v>-0.36174646472248362</v>
+        <f t="shared" si="11"/>
+        <v>0.33273753527751637</v>
       </c>
       <c r="E15">
-        <f t="shared" si="12"/>
-        <v>-0.23510015126050393</v>
+        <f t="shared" si="11"/>
+        <v>0.34837184873949606</v>
       </c>
       <c r="F15">
-        <f t="shared" si="12"/>
-        <v>-0.28457789108236908</v>
+        <f t="shared" si="11"/>
+        <v>0.25936010891763095</v>
       </c>
       <c r="G15">
-        <f t="shared" si="12"/>
-        <v>-0.2417127572427572</v>
+        <f t="shared" si="11"/>
+        <v>0.26275724275724277</v>
       </c>
       <c r="H15">
-        <f t="shared" si="12"/>
-        <v>-0.41468751777434276</v>
+        <f t="shared" si="11"/>
+        <v>0.24930448222565724</v>
       </c>
       <c r="I15">
-        <f t="shared" si="12"/>
-        <v>-3.5228882122174288E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.4462731178778257</v>
       </c>
       <c r="J15">
-        <f t="shared" si="12"/>
-        <v>-0.16606470588235306</v>
+        <f t="shared" si="11"/>
+        <v>0.38823529411764696</v>
       </c>
       <c r="K15">
-        <f t="shared" si="12"/>
-        <v>-0.24182666666666658</v>
+        <f t="shared" si="11"/>
+        <v>0.45833333333333343</v>
       </c>
       <c r="L15">
-        <f t="shared" si="12"/>
-        <v>-8.315084745762702E-2</v>
+        <f t="shared" si="11"/>
+        <v>0.55694915254237298</v>
       </c>
       <c r="M15">
-        <f t="shared" si="12"/>
-        <v>-0.22689920792079205</v>
+        <f t="shared" si="11"/>
+        <v>0.40792079207920789</v>
       </c>
       <c r="N15">
-        <f t="shared" si="12"/>
-        <v>-0.10660842105263146</v>
+        <f t="shared" si="11"/>
+        <v>0.55263157894736847</v>
       </c>
       <c r="O15">
-        <f t="shared" si="12"/>
-        <v>-0.33092672199170103</v>
+        <f t="shared" si="11"/>
+        <v>0.34481327800829897</v>
       </c>
       <c r="P15">
-        <f t="shared" si="12"/>
-        <v>-0.1497026262626262</v>
+        <f t="shared" si="11"/>
+        <v>0.42373737373737375</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="12"/>
-        <v>-0.23446623376623388</v>
+        <f t="shared" si="11"/>
+        <v>0.34623376623376612</v>
       </c>
       <c r="R15">
-        <f t="shared" si="12"/>
-        <v>-0.21408916890080432</v>
+        <f t="shared" si="11"/>
+        <v>0.37453083109919572</v>
       </c>
       <c r="S15">
-        <f t="shared" si="12"/>
-        <v>-0.34313360594795533</v>
+        <f t="shared" si="11"/>
+        <v>0.31412639405204462</v>
       </c>
       <c r="T15">
-        <f t="shared" si="12"/>
-        <v>-0.25244784313725488</v>
+        <f t="shared" si="11"/>
+        <v>0.38039215686274508</v>
       </c>
       <c r="U15">
-        <f t="shared" si="12"/>
-        <v>-0.56054782608695652</v>
+        <f t="shared" si="11"/>
+        <v>-2.9347826086956554E-2</v>
       </c>
       <c r="V15">
-        <f t="shared" si="12"/>
-        <v>-0.15884069498069497</v>
+        <f t="shared" si="11"/>
+        <v>0.50501930501930503</v>
       </c>
       <c r="W15">
-        <f t="shared" si="12"/>
-        <v>-0.20977745019920324</v>
+        <f t="shared" si="11"/>
+        <v>0.45936254980079672</v>
       </c>
       <c r="X15">
-        <f t="shared" si="12"/>
-        <v>-0.30269087533156497</v>
+        <f t="shared" si="11"/>
+        <v>0.28328912466843498</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="12"/>
-        <v>-0.13448884955752205</v>
+        <f t="shared" si="11"/>
+        <v>0.40199115044247791</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="12"/>
-        <v>-0.33626113821138209</v>
+        <f t="shared" si="11"/>
+        <v>0.33617886178861783</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="12"/>
-        <v>-0.34577295154185028</v>
+        <f t="shared" si="11"/>
+        <v>0.33920704845814975</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="12"/>
-        <v>-0.22720485981308419</v>
+        <f t="shared" si="11"/>
+        <v>0.46635514018691576</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="12"/>
-        <v>-0.17574000000000001</v>
+        <f t="shared" si="11"/>
+        <v>0.5</v>
       </c>
       <c r="AE15">
         <f t="shared" si="3"/>
@@ -15819,124 +16855,124 @@
       </c>
       <c r="AH15">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.33092672199170103</v>
+        <v>0.34481327800829897</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:I16" si="13">B4*-0.0081+0.8982+B10*0.0188-0.7434</f>
-        <v>0.70434100000000022</v>
+        <f t="shared" ref="B16:AC16" si="12">B15-((-0.0066*B5)+0.8348)</f>
+        <v>-5.779072800972862E-2</v>
       </c>
       <c r="C16">
-        <f t="shared" si="13"/>
-        <v>0.55995300000000003</v>
+        <f t="shared" si="12"/>
+        <v>-0.23399384687367081</v>
       </c>
       <c r="D16">
-        <f t="shared" si="13"/>
-        <v>0.62517800000000012</v>
+        <f t="shared" si="12"/>
+        <v>-0.36174646472248362</v>
       </c>
       <c r="E16">
-        <f t="shared" si="13"/>
-        <v>0.61884400000000006</v>
+        <f t="shared" si="12"/>
+        <v>-0.23510015126050393</v>
       </c>
       <c r="F16">
-        <f t="shared" si="13"/>
-        <v>0.44944100000000009</v>
+        <f t="shared" si="12"/>
+        <v>-0.28457789108236908</v>
       </c>
       <c r="G16">
-        <f t="shared" si="13"/>
-        <v>0.38539900000000016</v>
+        <f t="shared" si="12"/>
+        <v>-0.2417127572427572</v>
       </c>
       <c r="H16">
-        <f t="shared" si="13"/>
-        <v>0.4052079999999999</v>
+        <f t="shared" si="12"/>
+        <v>-0.41468751777434276</v>
       </c>
       <c r="I16">
-        <f t="shared" si="13"/>
-        <v>0.52265100000000009</v>
+        <f t="shared" si="12"/>
+        <v>-3.5228882122174288E-2</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:AC16" si="14">J4*-0.0081+0.8982+J10*0.0188-0.7434</f>
-        <v>0.50239</v>
+        <f t="shared" si="12"/>
+        <v>-0.16606470588235306</v>
       </c>
       <c r="K16">
-        <f t="shared" si="14"/>
-        <v>0.67764000000000013</v>
+        <f t="shared" si="12"/>
+        <v>-0.24182666666666658</v>
       </c>
       <c r="L16">
-        <f t="shared" si="14"/>
-        <v>0.68852999999999998</v>
+        <f t="shared" si="12"/>
+        <v>-8.315084745762702E-2</v>
       </c>
       <c r="M16">
-        <f t="shared" si="14"/>
-        <v>0.56737000000000026</v>
+        <f t="shared" si="12"/>
+        <v>-0.22689920792079205</v>
       </c>
       <c r="N16">
-        <f t="shared" si="14"/>
-        <v>0.69698000000000004</v>
+        <f t="shared" si="12"/>
+        <v>-0.10660842105263146</v>
       </c>
       <c r="O16">
-        <f t="shared" si="14"/>
-        <v>0.56495000000000017</v>
+        <f t="shared" si="12"/>
+        <v>-0.33092672199170103</v>
       </c>
       <c r="P16">
-        <f t="shared" si="14"/>
-        <v>0.64432000000000011</v>
+        <f t="shared" si="12"/>
+        <v>-0.1497026262626262</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="14"/>
-        <v>0.57803000000000015</v>
+        <f t="shared" si="12"/>
+        <v>-0.23446623376623388</v>
       </c>
       <c r="R16">
-        <f t="shared" si="14"/>
-        <v>0.57271000000000016</v>
+        <f t="shared" si="12"/>
+        <v>-0.21408916890080432</v>
       </c>
       <c r="S16">
-        <f t="shared" si="14"/>
-        <v>0.4614299999999999</v>
+        <f t="shared" si="12"/>
+        <v>-0.34313360594795533</v>
       </c>
       <c r="T16">
-        <f t="shared" si="14"/>
-        <v>0.64014000000000004</v>
+        <f t="shared" si="12"/>
+        <v>-0.25244784313725488</v>
       </c>
       <c r="U16">
-        <f t="shared" si="14"/>
-        <v>0.51352000000000009</v>
+        <f t="shared" si="12"/>
+        <v>-0.56054782608695652</v>
       </c>
       <c r="V16">
-        <f t="shared" si="14"/>
-        <v>0.59924999999999995</v>
+        <f t="shared" si="12"/>
+        <v>-0.15884069498069497</v>
       </c>
       <c r="W16">
-        <f t="shared" si="14"/>
-        <v>0.60572999999999999</v>
+        <f t="shared" si="12"/>
+        <v>-0.20977745019920324</v>
       </c>
       <c r="X16">
-        <f t="shared" si="14"/>
-        <v>0.78755000000000008</v>
+        <f t="shared" si="12"/>
+        <v>-0.30269087533156497</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="14"/>
-        <v>0.55196000000000012</v>
+        <f t="shared" si="12"/>
+        <v>-0.13448884955752205</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="14"/>
-        <v>0.6097800000000001</v>
+        <f t="shared" si="12"/>
+        <v>-0.33626113821138209</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="14"/>
-        <v>0.51424999999999998</v>
+        <f t="shared" si="12"/>
+        <v>-0.34577295154185028</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="14"/>
-        <v>0.58494000000000013</v>
+        <f t="shared" si="12"/>
+        <v>-0.22720485981308419</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="14"/>
-        <v>0.67775000000000019</v>
+        <f t="shared" si="12"/>
+        <v>-0.17574000000000001</v>
       </c>
       <c r="AE16">
         <f t="shared" si="3"/>
@@ -15952,10 +16988,129 @@
       </c>
       <c r="AH16">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.1497026262626262</v>
+        <v>0.42373737373737375</v>
       </c>
     </row>
-    <row r="17" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <f>B5*-0.00788+0.243179+B11*0.010781</f>
+        <v>0.47851006000000007</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:AD17" si="13">C5*-0.00788+0.243179+C11*0.010781</f>
+        <v>0.39946228000000006</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="13"/>
+        <v>0.44414478000000002</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="13"/>
+        <v>0.38609989000000011</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="13"/>
+        <v>0.26957686000000003</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="13"/>
+        <v>0.21350623000000005</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="13"/>
+        <v>0.30305567</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="13"/>
+        <v>0.28095663000000004</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="13"/>
+        <v>0.30501980000000006</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="13"/>
+        <v>0.47701160000000009</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="13"/>
+        <v>0.4538181</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="13"/>
+        <v>0.38175000000000003</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="13"/>
+        <v>0.4680453</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="13"/>
+        <v>0.40041920000000009</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="13"/>
+        <v>0.39579210000000009</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="13"/>
+        <v>0.36133610000000005</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="13"/>
+        <v>0.36216730000000008</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="13"/>
+        <v>0.33199690000000004</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="13"/>
+        <v>0.42251000000000005</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="13"/>
+        <v>0.30007990000000007</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="13"/>
+        <v>0.41426580000000002</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="13"/>
+        <v>0.42056979999999999</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="13"/>
+        <v>0.48407490000000009</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="13"/>
+        <v>0.3247116000000001</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="13"/>
+        <v>0.42450979999999994</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="13"/>
+        <v>0.37587389999999998</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="13"/>
+        <v>0.42061710000000008</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="13"/>
+        <v>0.4651052</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="13"/>
+        <v>0.48993890000000007</v>
+      </c>
       <c r="AE17">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -15970,10 +17125,10 @@
       </c>
       <c r="AH17">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.23446623376623388</v>
+        <v>0.34623376623376612</v>
       </c>
     </row>
-    <row r="18" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE18">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -15988,10 +17143,10 @@
       </c>
       <c r="AH18">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.21408916890080432</v>
+        <v>0.37453083109919572</v>
       </c>
     </row>
-    <row r="19" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE19">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -16006,10 +17161,10 @@
       </c>
       <c r="AH19">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.34313360594795533</v>
+        <v>0.31412639405204462</v>
       </c>
     </row>
-    <row r="20" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE20">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -16024,10 +17179,10 @@
       </c>
       <c r="AH20">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.25244784313725488</v>
+        <v>0.38039215686274508</v>
       </c>
     </row>
-    <row r="21" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE21">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -16042,10 +17197,10 @@
       </c>
       <c r="AH21">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.56054782608695652</v>
+        <v>-2.9347826086956554E-2</v>
       </c>
     </row>
-    <row r="22" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE22">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -16060,10 +17215,10 @@
       </c>
       <c r="AH22">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.15884069498069497</v>
+        <v>0.50501930501930503</v>
       </c>
     </row>
-    <row r="23" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE23">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -16078,10 +17233,10 @@
       </c>
       <c r="AH23">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.20977745019920324</v>
+        <v>0.45936254980079672</v>
       </c>
     </row>
-    <row r="24" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE24">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -16096,10 +17251,10 @@
       </c>
       <c r="AH24">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.30269087533156497</v>
+        <v>0.28328912466843498</v>
       </c>
     </row>
-    <row r="25" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE25">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -16114,10 +17269,10 @@
       </c>
       <c r="AH25">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.13448884955752205</v>
+        <v>0.40199115044247791</v>
       </c>
     </row>
-    <row r="26" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE26">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -16132,10 +17287,10 @@
       </c>
       <c r="AH26">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.33626113821138209</v>
+        <v>0.33617886178861783</v>
       </c>
     </row>
-    <row r="27" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE27">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -16150,10 +17305,10 @@
       </c>
       <c r="AH27">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.34577295154185028</v>
+        <v>0.33920704845814975</v>
       </c>
     </row>
-    <row r="28" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE28">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -16168,10 +17323,10 @@
       </c>
       <c r="AH28">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.22720485981308419</v>
+        <v>0.46635514018691576</v>
       </c>
     </row>
-    <row r="29" spans="31:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AE29">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -16186,10 +17341,11 @@
       </c>
       <c r="AH29">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.17574000000000001</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for Grey independent and other adjustments
</commit_message>
<xml_diff>
--- a/Ind-major preferencing.xlsx
+++ b/Ind-major preferencing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAE8AD2-66AE-4039-A35F-ACA5DB3393C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A52DC-8A27-4737-9413-EB0BA092C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="4725" windowWidth="19800" windowHeight="14655" firstSheet="1" activeTab="3" xr2:uid="{A68543AE-A11D-4AA7-B656-18DD4E512950}"/>
+    <workbookView xWindow="4995" yWindow="7395" windowWidth="19800" windowHeight="11475" firstSheet="1" activeTab="3" xr2:uid="{A68543AE-A11D-4AA7-B656-18DD4E512950}"/>
   </bookViews>
   <sheets>
     <sheet name="LNP seat regression" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -14179,7 +14180,7 @@
         <v>0.66861000000000004</v>
       </c>
       <c r="CL17">
-        <f t="shared" ref="CL17:CX17" si="27">CL5*-0.0081+0.8982+CL11*0.0188-0.7434</f>
+        <f t="shared" ref="CL17:CT17" si="27">CL5*-0.0081+0.8982+CL11*0.0188-0.7434</f>
         <v>0.40631000000000006</v>
       </c>
       <c r="CM17">
@@ -15743,7 +15744,7 @@
         <v>23.8</v>
       </c>
       <c r="AE4">
-        <f t="shared" ref="AE4:AE30" si="3">AE3+1</f>
+        <f t="shared" ref="AE4:AE29" si="3">AE3+1</f>
         <v>2</v>
       </c>
       <c r="AF4">

</xml_diff>